<commit_message>
Changed simulation to use daily returns instead of monthly returns (up to tildes); removed redundant/unused code
</commit_message>
<xml_diff>
--- a/returns_correlation_matrix.xlsx
+++ b/returns_correlation_matrix.xlsx
@@ -539,91 +539,91 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0455</v>
+        <v>0.1652</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5377</v>
+        <v>0.4105</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2688</v>
+        <v>0.24</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3792</v>
+        <v>0.2862</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4468</v>
+        <v>0.3827</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.0247</v>
+        <v>0.0789</v>
       </c>
       <c r="I2" t="n">
-        <v>0.039</v>
+        <v>0.174</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1805</v>
+        <v>0.1666</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2558</v>
+        <v>0.1996</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4312</v>
+        <v>0.3357</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1909</v>
+        <v>0.2259</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1</v>
+        <v>0.197</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2299</v>
+        <v>0.1989</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0701</v>
+        <v>0.1755</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.1675</v>
+        <v>0.2129</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0675</v>
+        <v>0.0694</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0883</v>
+        <v>0.0009</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0039</v>
+        <v>0.167</v>
       </c>
       <c r="U2" t="n">
-        <v>0.2532</v>
+        <v>0.2834</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1384</v>
+        <v>0.1515</v>
       </c>
       <c r="W2" t="n">
-        <v>0.3403</v>
+        <v>0.2907</v>
       </c>
       <c r="X2" t="n">
-        <v>0.2818</v>
+        <v>0.3097</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.4052</v>
+        <v>0.2859</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.3234</v>
+        <v>0.2748</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.239</v>
+        <v>0.1411</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.1156</v>
+        <v>0.2543</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.2519</v>
+        <v>0.2441</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.0545</v>
+        <v>-0.0433</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.1169</v>
+        <v>-0.2017</v>
       </c>
     </row>
     <row r="3">
@@ -631,94 +631,94 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.0455</v>
+        <v>0.1652</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.061</v>
+        <v>0.2183</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0182</v>
+        <v>0.0836</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0558</v>
+        <v>0.1721</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0688</v>
+        <v>0.1745</v>
       </c>
       <c r="H3" t="n">
-        <v>0.1766</v>
+        <v>0.1019</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2351</v>
+        <v>0.1437</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2182</v>
+        <v>0.0874</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1143</v>
+        <v>0.1132</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0584</v>
+        <v>0.1543</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.0052</v>
+        <v>0.114</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.0675</v>
+        <v>0.107</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1143</v>
+        <v>0.1134</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1909</v>
+        <v>0.2154</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1974</v>
+        <v>0.1678</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0688</v>
+        <v>0.1001</v>
       </c>
       <c r="S3" t="n">
-        <v>-0.113</v>
+        <v>-0.0162</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1792</v>
+        <v>0.1395</v>
       </c>
       <c r="U3" t="n">
-        <v>0.013</v>
+        <v>0.0853</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1072</v>
+        <v>0.0813</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0429</v>
+        <v>0.1277</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1169</v>
+        <v>0.1185</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.0351</v>
+        <v>0.1258</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.1299</v>
+        <v>0.1632</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.0039</v>
+        <v>0.1167</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1065</v>
+        <v>0.1642</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1156</v>
+        <v>0.1313</v>
       </c>
       <c r="AD3" t="n">
-        <v>-0.2039</v>
+        <v>-0.0117</v>
       </c>
       <c r="AE3" t="n">
-        <v>-0.0325</v>
+        <v>-0.0855</v>
       </c>
     </row>
     <row r="4">
@@ -726,94 +726,94 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5377</v>
+        <v>0.4105</v>
       </c>
       <c r="C4" t="n">
-        <v>0.061</v>
+        <v>0.2183</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3364</v>
+        <v>0.2336</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4182</v>
+        <v>0.3281</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5039</v>
+        <v>0.5043</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1026</v>
+        <v>0.1078</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1532</v>
+        <v>0.2314</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2844</v>
+        <v>0.2549</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2766</v>
+        <v>0.2276</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3974</v>
+        <v>0.4364</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0922</v>
+        <v>0.2166</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1208</v>
+        <v>0.2687</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2792</v>
+        <v>0.2554</v>
       </c>
       <c r="P4" t="n">
-        <v>0.2312</v>
+        <v>0.2418</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.2688</v>
+        <v>0.2416</v>
       </c>
       <c r="R4" t="n">
-        <v>-0.0312</v>
+        <v>0.0875</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0078</v>
+        <v>0.0471</v>
       </c>
       <c r="T4" t="n">
-        <v>0.1364</v>
+        <v>0.2149</v>
       </c>
       <c r="U4" t="n">
-        <v>0.2714</v>
+        <v>0.3014</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1955</v>
+        <v>0.1159</v>
       </c>
       <c r="W4" t="n">
-        <v>0.3195</v>
+        <v>0.3596</v>
       </c>
       <c r="X4" t="n">
-        <v>0.3494</v>
+        <v>0.3619</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.4078</v>
+        <v>0.314</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.3701</v>
+        <v>0.3124</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.1766</v>
+        <v>0.2206</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.2688</v>
+        <v>0.3089</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.2727</v>
+        <v>0.2833</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.0364</v>
+        <v>-0.0187</v>
       </c>
       <c r="AE4" t="n">
-        <v>-0.1662</v>
+        <v>-0.226</v>
       </c>
     </row>
     <row r="5">
@@ -821,94 +821,94 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2688</v>
+        <v>0.24</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0182</v>
+        <v>0.0836</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3364</v>
+        <v>0.2336</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3416</v>
+        <v>0.2039</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1831</v>
+        <v>0.2208</v>
       </c>
       <c r="H5" t="n">
-        <v>0.187</v>
+        <v>0.1093</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2818</v>
+        <v>0.1887</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2286</v>
+        <v>0.1878</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0519</v>
+        <v>0.1535</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1779</v>
+        <v>0.2478</v>
       </c>
       <c r="M5" t="n">
-        <v>0.039</v>
+        <v>0.1262</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1974</v>
+        <v>0.1842</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2649</v>
+        <v>0.2031</v>
       </c>
       <c r="P5" t="n">
-        <v>0.1649</v>
+        <v>0.1774</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.0104</v>
+        <v>0.1134</v>
       </c>
       <c r="R5" t="n">
-        <v>-0.061</v>
+        <v>0.0693</v>
       </c>
       <c r="S5" t="n">
-        <v>-0.0948</v>
+        <v>0.0118</v>
       </c>
       <c r="T5" t="n">
-        <v>0.1896</v>
+        <v>0.1697</v>
       </c>
       <c r="U5" t="n">
-        <v>0.1584</v>
+        <v>0.181</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.0604</v>
+        <v>0.0344</v>
       </c>
       <c r="W5" t="n">
-        <v>0.2636</v>
+        <v>0.2716</v>
       </c>
       <c r="X5" t="n">
-        <v>0.2312</v>
+        <v>0.268</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.2532</v>
+        <v>0.1899</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.3221</v>
+        <v>0.3158</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.1857</v>
+        <v>0.1709</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.1091</v>
+        <v>0.1821</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.1675</v>
+        <v>0.1863</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.1208</v>
+        <v>0.0184</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.0065</v>
+        <v>-0.0845</v>
       </c>
     </row>
     <row r="6">
@@ -916,94 +916,94 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.3792</v>
+        <v>0.2862</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0558</v>
+        <v>0.1721</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4182</v>
+        <v>0.3281</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3416</v>
+        <v>0.2039</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2727</v>
+        <v>0.2731</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1078</v>
+        <v>0.1066</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0805</v>
+        <v>0.2063</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3312</v>
+        <v>0.2296</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1545</v>
+        <v>0.1716</v>
       </c>
       <c r="L6" t="n">
-        <v>0.3195</v>
+        <v>0.2999</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0948</v>
+        <v>0.2115</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2247</v>
+        <v>0.2409</v>
       </c>
       <c r="O6" t="n">
-        <v>0.2221</v>
+        <v>0.2233</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1299</v>
+        <v>0.1779</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1961</v>
+        <v>0.1795</v>
       </c>
       <c r="R6" t="n">
-        <v>0.0805</v>
+        <v>0.0989</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.0753</v>
+        <v>-0.0029</v>
       </c>
       <c r="T6" t="n">
-        <v>0.1545</v>
+        <v>0.1794</v>
       </c>
       <c r="U6" t="n">
-        <v>0.3883</v>
+        <v>0.2869</v>
       </c>
       <c r="V6" t="n">
-        <v>0.141</v>
+        <v>0.0856</v>
       </c>
       <c r="W6" t="n">
-        <v>0.3636</v>
+        <v>0.3568</v>
       </c>
       <c r="X6" t="n">
-        <v>0.3909</v>
+        <v>0.4037</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.3792</v>
+        <v>0.2419</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.1935</v>
+        <v>0.2681</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.2</v>
+        <v>0.1852</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.2766</v>
+        <v>0.2251</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.2857</v>
+        <v>0.2996</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.0545</v>
+        <v>-0.0009</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.0494</v>
+        <v>-0.1158</v>
       </c>
     </row>
     <row r="7">
@@ -1011,94 +1011,94 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4468</v>
+        <v>0.3827</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0688</v>
+        <v>0.1745</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5039</v>
+        <v>0.5043</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1831</v>
+        <v>0.2208</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2727</v>
+        <v>0.2731</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.0247</v>
+        <v>0.0619</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1247</v>
+        <v>0.1294</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1597</v>
+        <v>0.1641</v>
       </c>
       <c r="K7" t="n">
-        <v>0.2247</v>
+        <v>0.2078</v>
       </c>
       <c r="L7" t="n">
-        <v>0.4416</v>
+        <v>0.4317</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1078</v>
+        <v>0.1879</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0117</v>
+        <v>0.1807</v>
       </c>
       <c r="O7" t="n">
-        <v>0.2299</v>
+        <v>0.237</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0727</v>
+        <v>0.1585</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.2792</v>
+        <v>0.2359</v>
       </c>
       <c r="R7" t="n">
-        <v>-0.0338</v>
+        <v>0.0204</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0026</v>
+        <v>0.0785</v>
       </c>
       <c r="T7" t="n">
-        <v>0.0247</v>
+        <v>0.1805</v>
       </c>
       <c r="U7" t="n">
-        <v>0.1208</v>
+        <v>0.2491</v>
       </c>
       <c r="V7" t="n">
-        <v>0.1773</v>
+        <v>0.1137</v>
       </c>
       <c r="W7" t="n">
-        <v>0.1558</v>
+        <v>0.2727</v>
       </c>
       <c r="X7" t="n">
-        <v>0.2143</v>
+        <v>0.274</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.2987</v>
+        <v>0.2994</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.2662</v>
+        <v>0.2682</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.0597</v>
+        <v>0.1765</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.1935</v>
+        <v>0.2359</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.1532</v>
+        <v>0.2063</v>
       </c>
       <c r="AD7" t="n">
-        <v>-0.1948</v>
+        <v>-0.1061</v>
       </c>
       <c r="AE7" t="n">
-        <v>-0.3065</v>
+        <v>-0.3089</v>
       </c>
     </row>
     <row r="8">
@@ -1106,94 +1106,94 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.0247</v>
+        <v>0.0789</v>
       </c>
       <c r="C8" t="n">
-        <v>0.1766</v>
+        <v>0.1019</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1026</v>
+        <v>0.1078</v>
       </c>
       <c r="E8" t="n">
-        <v>0.187</v>
+        <v>0.1093</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1078</v>
+        <v>0.1066</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.0247</v>
+        <v>0.0619</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2325</v>
+        <v>0.3408</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1766</v>
+        <v>0.1547</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.013</v>
+        <v>0.1198</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0221</v>
+        <v>0.0512</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0052</v>
+        <v>0.0413</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0338</v>
+        <v>0.1173</v>
       </c>
       <c r="O8" t="n">
-        <v>0.0286</v>
+        <v>0.1226</v>
       </c>
       <c r="P8" t="n">
-        <v>0.1468</v>
+        <v>0.2563</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.0701</v>
+        <v>0.1062</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.0195</v>
+        <v>0.1458</v>
       </c>
       <c r="S8" t="n">
-        <v>0.0455</v>
+        <v>-0.0085</v>
       </c>
       <c r="T8" t="n">
-        <v>0.239</v>
+        <v>0.1533</v>
       </c>
       <c r="U8" t="n">
-        <v>0.0779</v>
+        <v>0.0331</v>
       </c>
       <c r="V8" t="n">
-        <v>-0.1163</v>
+        <v>-0.0072</v>
       </c>
       <c r="W8" t="n">
-        <v>0.0532</v>
+        <v>0.0255</v>
       </c>
       <c r="X8" t="n">
-        <v>0.0571</v>
+        <v>0.059</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.0117</v>
+        <v>0.0721</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.0779</v>
+        <v>0.1259</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.0013</v>
+        <v>0.1499</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.0753</v>
+        <v>0.097</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.1182</v>
+        <v>-0.0112</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.0636</v>
+        <v>0.0059</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.0195</v>
+        <v>-0.0088</v>
       </c>
     </row>
     <row r="9">
@@ -1201,94 +1201,94 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.039</v>
+        <v>0.174</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2351</v>
+        <v>0.1437</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1532</v>
+        <v>0.2314</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2818</v>
+        <v>0.1887</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0805</v>
+        <v>0.2063</v>
       </c>
       <c r="G9" t="n">
-        <v>0.1247</v>
+        <v>0.1294</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2325</v>
+        <v>0.3408</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3</v>
+        <v>0.2362</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0688</v>
+        <v>0.1681</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1065</v>
+        <v>0.1805</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0974</v>
+        <v>0.0806</v>
       </c>
       <c r="N9" t="n">
-        <v>0.2584</v>
+        <v>0.2169</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1883</v>
+        <v>0.2183</v>
       </c>
       <c r="P9" t="n">
-        <v>0.0987</v>
+        <v>0.3095</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.0688</v>
+        <v>0.136</v>
       </c>
       <c r="R9" t="n">
-        <v>0.0909</v>
+        <v>0.1975</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.1844</v>
+        <v>-0.0405</v>
       </c>
       <c r="T9" t="n">
-        <v>0.1208</v>
+        <v>0.2313</v>
       </c>
       <c r="U9" t="n">
-        <v>0.0532</v>
+        <v>0.1303</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.1591</v>
+        <v>0.0164</v>
       </c>
       <c r="W9" t="n">
-        <v>0.2519</v>
+        <v>0.2309</v>
       </c>
       <c r="X9" t="n">
-        <v>0.2532</v>
+        <v>0.2134</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.2753</v>
+        <v>0.1775</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.1286</v>
+        <v>0.2507</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.2078</v>
+        <v>0.2459</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1597</v>
+        <v>0.1837</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.3039</v>
+        <v>0.1307</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.0234</v>
+        <v>0.0275</v>
       </c>
       <c r="AE9" t="n">
-        <v>-0.026</v>
+        <v>-0.0177</v>
       </c>
     </row>
     <row r="10">
@@ -1296,94 +1296,94 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1805</v>
+        <v>0.1666</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2182</v>
+        <v>0.0874</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2844</v>
+        <v>0.2549</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2286</v>
+        <v>0.1878</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3312</v>
+        <v>0.2296</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1597</v>
+        <v>0.1641</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1766</v>
+        <v>0.1547</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3</v>
+        <v>0.2362</v>
       </c>
       <c r="J10" t="n">
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>0.013</v>
+        <v>0.0987</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1935</v>
+        <v>0.2121</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1403</v>
+        <v>0.1533</v>
       </c>
       <c r="N10" t="n">
-        <v>0.3195</v>
+        <v>0.2876</v>
       </c>
       <c r="O10" t="n">
-        <v>0.3714</v>
+        <v>0.3561</v>
       </c>
       <c r="P10" t="n">
-        <v>0.1156</v>
+        <v>0.164</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.1584</v>
+        <v>0.0964</v>
       </c>
       <c r="R10" t="n">
-        <v>0.113</v>
+        <v>0.0878</v>
       </c>
       <c r="S10" t="n">
-        <v>-0.0481</v>
+        <v>-0.0203</v>
       </c>
       <c r="T10" t="n">
-        <v>0.2234</v>
+        <v>0.1748</v>
       </c>
       <c r="U10" t="n">
-        <v>0.2519</v>
+        <v>0.1333</v>
       </c>
       <c r="V10" t="n">
-        <v>0.0994</v>
+        <v>0.0395</v>
       </c>
       <c r="W10" t="n">
-        <v>0.2377</v>
+        <v>0.2111</v>
       </c>
       <c r="X10" t="n">
-        <v>0.2649</v>
+        <v>0.2185</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.1961</v>
+        <v>0.1093</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.1792</v>
+        <v>0.1929</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.274</v>
+        <v>0.3356</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.1662</v>
+        <v>0.1573</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.2429</v>
+        <v>0.1206</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.1597</v>
+        <v>0.0174</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.0818</v>
+        <v>-0.0223</v>
       </c>
     </row>
     <row r="11">
@@ -1391,94 +1391,94 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2558</v>
+        <v>0.1996</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1143</v>
+        <v>0.1132</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2766</v>
+        <v>0.2276</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0519</v>
+        <v>0.1535</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1545</v>
+        <v>0.1716</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2247</v>
+        <v>0.2078</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.013</v>
+        <v>0.1198</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.0688</v>
+        <v>0.1681</v>
       </c>
       <c r="J11" t="n">
-        <v>0.013</v>
+        <v>0.0987</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2325</v>
+        <v>0.1894</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1662</v>
+        <v>0.1122</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0416</v>
+        <v>0.1743</v>
       </c>
       <c r="O11" t="n">
-        <v>0</v>
+        <v>0.0788</v>
       </c>
       <c r="P11" t="n">
-        <v>0.1494</v>
+        <v>0.1745</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.3117</v>
+        <v>0.2106</v>
       </c>
       <c r="R11" t="n">
-        <v>0.2221</v>
+        <v>0.1734</v>
       </c>
       <c r="S11" t="n">
-        <v>0.0403</v>
+        <v>0.024</v>
       </c>
       <c r="T11" t="n">
-        <v>0.0208</v>
+        <v>0.1138</v>
       </c>
       <c r="U11" t="n">
-        <v>0.1844</v>
+        <v>0.1654</v>
       </c>
       <c r="V11" t="n">
-        <v>0.254</v>
+        <v>0.0718</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0844</v>
+        <v>0.1604</v>
       </c>
       <c r="X11" t="n">
-        <v>0.0987</v>
+        <v>0.1727</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.2481</v>
+        <v>0.187</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.1195</v>
+        <v>0.2165</v>
       </c>
       <c r="AA11" t="n">
-        <v>-0.0195</v>
+        <v>0.0843</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.1558</v>
+        <v>0.2031</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.1623</v>
+        <v>0.1599</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.0584</v>
+        <v>0.0351</v>
       </c>
       <c r="AE11" t="n">
-        <v>-0.0143</v>
+        <v>-0.0313</v>
       </c>
     </row>
     <row r="12">
@@ -1486,94 +1486,94 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4312</v>
+        <v>0.3357</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0584</v>
+        <v>0.1543</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3974</v>
+        <v>0.4364</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1779</v>
+        <v>0.2478</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3195</v>
+        <v>0.2999</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4416</v>
+        <v>0.4317</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.0221</v>
+        <v>0.0512</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1065</v>
+        <v>0.1805</v>
       </c>
       <c r="J12" t="n">
-        <v>0.1935</v>
+        <v>0.2121</v>
       </c>
       <c r="K12" t="n">
-        <v>0.2325</v>
+        <v>0.1894</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>0.1182</v>
+        <v>0.1931</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0636</v>
+        <v>0.2506</v>
       </c>
       <c r="O12" t="n">
-        <v>0.2481</v>
+        <v>0.2502</v>
       </c>
       <c r="P12" t="n">
-        <v>0.1766</v>
+        <v>0.1958</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.2896</v>
+        <v>0.1956</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0026</v>
+        <v>0.096</v>
       </c>
       <c r="S12" t="n">
-        <v>0.0052</v>
+        <v>0.0652</v>
       </c>
       <c r="T12" t="n">
-        <v>-0.0039</v>
+        <v>0.2096</v>
       </c>
       <c r="U12" t="n">
-        <v>0.0844</v>
+        <v>0.2751</v>
       </c>
       <c r="V12" t="n">
-        <v>0.1669</v>
+        <v>0.1103</v>
       </c>
       <c r="W12" t="n">
-        <v>0.2935</v>
+        <v>0.3848</v>
       </c>
       <c r="X12" t="n">
-        <v>0.2506</v>
+        <v>0.3563</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.4026</v>
+        <v>0.2967</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.2325</v>
+        <v>0.2938</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.1636</v>
+        <v>0.1898</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.1961</v>
+        <v>0.2595</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.1948</v>
+        <v>0.2772</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.026</v>
+        <v>-0.03</v>
       </c>
       <c r="AE12" t="n">
-        <v>-0.1455</v>
+        <v>-0.2095</v>
       </c>
     </row>
     <row r="13">
@@ -1581,94 +1581,94 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.1909</v>
+        <v>0.2259</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0052</v>
+        <v>0.114</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0922</v>
+        <v>0.2166</v>
       </c>
       <c r="E13" t="n">
-        <v>0.039</v>
+        <v>0.1262</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0948</v>
+        <v>0.2115</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1078</v>
+        <v>0.1879</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0052</v>
+        <v>0.0413</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0974</v>
+        <v>0.0806</v>
       </c>
       <c r="J13" t="n">
-        <v>0.1403</v>
+        <v>0.1533</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1662</v>
+        <v>0.1122</v>
       </c>
       <c r="L13" t="n">
-        <v>0.1182</v>
+        <v>0.1931</v>
       </c>
       <c r="M13" t="n">
         <v>1</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2727</v>
+        <v>0.2242</v>
       </c>
       <c r="O13" t="n">
-        <v>0.3065</v>
+        <v>0.1976</v>
       </c>
       <c r="P13" t="n">
-        <v>-0.0403</v>
+        <v>0.1078</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0338</v>
+        <v>0.1637</v>
       </c>
       <c r="R13" t="n">
-        <v>0.1909</v>
+        <v>0.0877</v>
       </c>
       <c r="S13" t="n">
-        <v>0.1078</v>
+        <v>0.0249</v>
       </c>
       <c r="T13" t="n">
-        <v>-0.0442</v>
+        <v>0.1095</v>
       </c>
       <c r="U13" t="n">
-        <v>0.0779</v>
+        <v>0.1813</v>
       </c>
       <c r="V13" t="n">
-        <v>0.1462</v>
+        <v>0.0819</v>
       </c>
       <c r="W13" t="n">
-        <v>0.1649</v>
+        <v>0.222</v>
       </c>
       <c r="X13" t="n">
-        <v>0.0494</v>
+        <v>0.2434</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.1519</v>
+        <v>0.1894</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.026</v>
+        <v>0.185</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.1468</v>
+        <v>0.1248</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.0675</v>
+        <v>0.1722</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.1468</v>
+        <v>0.2188</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.0948</v>
+        <v>-0.0154</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.0117</v>
+        <v>-0.1248</v>
       </c>
     </row>
     <row r="14">
@@ -1676,94 +1676,94 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1</v>
+        <v>0.197</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.0675</v>
+        <v>0.107</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1208</v>
+        <v>0.2687</v>
       </c>
       <c r="E14" t="n">
-        <v>0.1974</v>
+        <v>0.1842</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2247</v>
+        <v>0.2409</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0117</v>
+        <v>0.1807</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0338</v>
+        <v>0.1173</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2584</v>
+        <v>0.2169</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3195</v>
+        <v>0.2876</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0416</v>
+        <v>0.1743</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0636</v>
+        <v>0.2506</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2727</v>
+        <v>0.2242</v>
       </c>
       <c r="N14" t="n">
         <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>0.3143</v>
+        <v>0.2822</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0091</v>
+        <v>0.1728</v>
       </c>
       <c r="Q14" t="n">
-        <v>-0.0623</v>
+        <v>0.1153</v>
       </c>
       <c r="R14" t="n">
-        <v>0.2273</v>
+        <v>0.1667</v>
       </c>
       <c r="S14" t="n">
-        <v>-0.074</v>
+        <v>-0.0166</v>
       </c>
       <c r="T14" t="n">
-        <v>0.0779</v>
+        <v>0.1599</v>
       </c>
       <c r="U14" t="n">
-        <v>0.1922</v>
+        <v>0.221</v>
       </c>
       <c r="V14" t="n">
-        <v>-0.1046</v>
+        <v>0.0666</v>
       </c>
       <c r="W14" t="n">
-        <v>0.3052</v>
+        <v>0.3048</v>
       </c>
       <c r="X14" t="n">
-        <v>0.2104</v>
+        <v>0.3248</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.2377</v>
+        <v>0.1617</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.0442</v>
+        <v>0.2399</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.3545</v>
+        <v>0.2795</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.1896</v>
+        <v>0.2102</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.2532</v>
+        <v>0.2277</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.1468</v>
+        <v>0.0251</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.2195</v>
+        <v>-0.0283</v>
       </c>
     </row>
     <row r="15">
@@ -1771,94 +1771,94 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2299</v>
+        <v>0.1989</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1143</v>
+        <v>0.1134</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2792</v>
+        <v>0.2554</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2649</v>
+        <v>0.2031</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2221</v>
+        <v>0.2233</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2299</v>
+        <v>0.237</v>
       </c>
       <c r="H15" t="n">
-        <v>0.0286</v>
+        <v>0.1226</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1883</v>
+        <v>0.2183</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3714</v>
+        <v>0.3561</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>0.0788</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2481</v>
+        <v>0.2502</v>
       </c>
       <c r="M15" t="n">
-        <v>0.3065</v>
+        <v>0.1976</v>
       </c>
       <c r="N15" t="n">
-        <v>0.3143</v>
+        <v>0.2822</v>
       </c>
       <c r="O15" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>0.074</v>
+        <v>0.1618</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.187</v>
+        <v>0.1296</v>
       </c>
       <c r="R15" t="n">
-        <v>0.0922</v>
+        <v>0.1496</v>
       </c>
       <c r="S15" t="n">
-        <v>0.0169</v>
+        <v>0.0213</v>
       </c>
       <c r="T15" t="n">
-        <v>0.0052</v>
+        <v>0.1737</v>
       </c>
       <c r="U15" t="n">
-        <v>0.0052</v>
+        <v>0.1474</v>
       </c>
       <c r="V15" t="n">
-        <v>0.0552</v>
+        <v>0.1016</v>
       </c>
       <c r="W15" t="n">
-        <v>0.2403</v>
+        <v>0.2378</v>
       </c>
       <c r="X15" t="n">
-        <v>0.1688</v>
+        <v>0.2364</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.1597</v>
+        <v>0.1484</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.0857</v>
+        <v>0.2003</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.3675</v>
+        <v>0.388</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.1013</v>
+        <v>0.1541</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.2013</v>
+        <v>0.1594</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.0065</v>
+        <v>-0.0003</v>
       </c>
       <c r="AE15" t="n">
-        <v>-0.0377</v>
+        <v>-0.063</v>
       </c>
     </row>
     <row r="16">
@@ -1866,94 +1866,94 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0701</v>
+        <v>0.1755</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1909</v>
+        <v>0.2154</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2312</v>
+        <v>0.2418</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1649</v>
+        <v>0.1774</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1299</v>
+        <v>0.1779</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0727</v>
+        <v>0.1585</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1468</v>
+        <v>0.2563</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0987</v>
+        <v>0.3095</v>
       </c>
       <c r="J16" t="n">
-        <v>0.1156</v>
+        <v>0.164</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1494</v>
+        <v>0.1745</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1766</v>
+        <v>0.1958</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.0403</v>
+        <v>0.1078</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0091</v>
+        <v>0.1728</v>
       </c>
       <c r="O16" t="n">
-        <v>0.074</v>
+        <v>0.1618</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.2714</v>
+        <v>0.1514</v>
       </c>
       <c r="R16" t="n">
-        <v>0.0416</v>
+        <v>0.1796</v>
       </c>
       <c r="S16" t="n">
-        <v>-0.0519</v>
+        <v>-0.0183</v>
       </c>
       <c r="T16" t="n">
-        <v>0.2532</v>
+        <v>0.2332</v>
       </c>
       <c r="U16" t="n">
-        <v>0.1519</v>
+        <v>0.1216</v>
       </c>
       <c r="V16" t="n">
-        <v>0.1215</v>
+        <v>0.0424</v>
       </c>
       <c r="W16" t="n">
-        <v>0.1455</v>
+        <v>0.174</v>
       </c>
       <c r="X16" t="n">
-        <v>0.1935</v>
+        <v>0.1921</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.1818</v>
+        <v>0.1441</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.2948</v>
+        <v>0.2187</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.1377</v>
+        <v>0.1659</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.1701</v>
+        <v>0.1922</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.0649</v>
+        <v>0.1199</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.0571</v>
+        <v>-0.0434</v>
       </c>
       <c r="AE16" t="n">
-        <v>-0.0312</v>
+        <v>-0.0673</v>
       </c>
     </row>
     <row r="17">
@@ -1961,94 +1961,94 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1675</v>
+        <v>0.2129</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1974</v>
+        <v>0.1678</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2688</v>
+        <v>0.2416</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0104</v>
+        <v>0.1134</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1961</v>
+        <v>0.1795</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2792</v>
+        <v>0.2359</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0701</v>
+        <v>0.1062</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0688</v>
+        <v>0.136</v>
       </c>
       <c r="J17" t="n">
-        <v>0.1584</v>
+        <v>0.0964</v>
       </c>
       <c r="K17" t="n">
-        <v>0.3117</v>
+        <v>0.2106</v>
       </c>
       <c r="L17" t="n">
-        <v>0.2896</v>
+        <v>0.1956</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0338</v>
+        <v>0.1637</v>
       </c>
       <c r="N17" t="n">
-        <v>-0.0623</v>
+        <v>0.1153</v>
       </c>
       <c r="O17" t="n">
-        <v>0.187</v>
+        <v>0.1296</v>
       </c>
       <c r="P17" t="n">
-        <v>0.2714</v>
+        <v>0.1514</v>
       </c>
       <c r="Q17" t="n">
         <v>1</v>
       </c>
       <c r="R17" t="n">
+        <v>0.1618</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.0183</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.1145</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.1579</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.1274</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.1587</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.1913</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.2282</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.1873</v>
+      </c>
+      <c r="AA17" t="n">
         <v>0.1104</v>
       </c>
-      <c r="S17" t="n">
-        <v>-0.1364</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0.1974</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.1299</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.2917</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0.113</v>
-      </c>
-      <c r="X17" t="n">
-        <v>0.1117</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>0.126</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>0.0714</v>
-      </c>
       <c r="AB17" t="n">
-        <v>0.1221</v>
+        <v>0.1826</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.1571</v>
+        <v>0.1843</v>
       </c>
       <c r="AD17" t="n">
-        <v>-0.1312</v>
+        <v>-0.0625</v>
       </c>
       <c r="AE17" t="n">
-        <v>-0.1545</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="18">
@@ -2056,94 +2056,94 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0675</v>
+        <v>0.0694</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0688</v>
+        <v>0.1001</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.0312</v>
+        <v>0.0875</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.061</v>
+        <v>0.0693</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0805</v>
+        <v>0.0989</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.0338</v>
+        <v>0.0204</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.0195</v>
+        <v>0.1458</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0909</v>
+        <v>0.1975</v>
       </c>
       <c r="J18" t="n">
-        <v>0.113</v>
+        <v>0.0878</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2221</v>
+        <v>0.1734</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.0026</v>
+        <v>0.096</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1909</v>
+        <v>0.0877</v>
       </c>
       <c r="N18" t="n">
-        <v>0.2273</v>
+        <v>0.1667</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0922</v>
+        <v>0.1496</v>
       </c>
       <c r="P18" t="n">
-        <v>0.0416</v>
+        <v>0.1796</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.1104</v>
+        <v>0.1618</v>
       </c>
       <c r="R18" t="n">
         <v>1</v>
       </c>
       <c r="S18" t="n">
-        <v>0.0338</v>
+        <v>-0.0147</v>
       </c>
       <c r="T18" t="n">
-        <v>-0.0377</v>
+        <v>0.0828</v>
       </c>
       <c r="U18" t="n">
-        <v>0.0792</v>
+        <v>0.0631</v>
       </c>
       <c r="V18" t="n">
-        <v>0.1072</v>
+        <v>0.0492</v>
       </c>
       <c r="W18" t="n">
-        <v>0.0675</v>
+        <v>0.1185</v>
       </c>
       <c r="X18" t="n">
-        <v>0.0584</v>
+        <v>0.1332</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.1948</v>
+        <v>0.1014</v>
       </c>
       <c r="Z18" t="n">
-        <v>-0.0532</v>
+        <v>0.1283</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.1974</v>
+        <v>0.1528</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.126</v>
+        <v>0.1122</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.0805</v>
+        <v>0.0961</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.0649</v>
+        <v>0.0497</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.2831</v>
+        <v>0.1188</v>
       </c>
     </row>
     <row r="19">
@@ -2151,94 +2151,94 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0883</v>
+        <v>0.0009</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.113</v>
+        <v>-0.0162</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0078</v>
+        <v>0.0471</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.0948</v>
+        <v>0.0118</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.0753</v>
+        <v>-0.0029</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0026</v>
+        <v>0.0785</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0455</v>
+        <v>-0.0085</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.1844</v>
+        <v>-0.0405</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0481</v>
+        <v>-0.0203</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0403</v>
+        <v>0.024</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0052</v>
+        <v>0.0652</v>
       </c>
       <c r="M19" t="n">
-        <v>0.1078</v>
+        <v>0.0249</v>
       </c>
       <c r="N19" t="n">
-        <v>-0.074</v>
+        <v>-0.0166</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0169</v>
+        <v>0.0213</v>
       </c>
       <c r="P19" t="n">
-        <v>-0.0519</v>
+        <v>-0.0183</v>
       </c>
       <c r="Q19" t="n">
-        <v>-0.1364</v>
+        <v>0.0183</v>
       </c>
       <c r="R19" t="n">
-        <v>0.0338</v>
+        <v>-0.0147</v>
       </c>
       <c r="S19" t="n">
         <v>1</v>
       </c>
       <c r="T19" t="n">
-        <v>-0.1052</v>
+        <v>-0.0124</v>
       </c>
       <c r="U19" t="n">
-        <v>-0.1857</v>
+        <v>-0.0406</v>
       </c>
       <c r="V19" t="n">
-        <v>0.0318</v>
+        <v>0.0567</v>
       </c>
       <c r="W19" t="n">
-        <v>-0.0286</v>
+        <v>0.009</v>
       </c>
       <c r="X19" t="n">
-        <v>-0.1442</v>
+        <v>-0.0038</v>
       </c>
       <c r="Y19" t="n">
-        <v>-0.0468</v>
+        <v>-0.0147</v>
       </c>
       <c r="Z19" t="n">
-        <v>-0.0714</v>
+        <v>0.0076</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.0312</v>
+        <v>-0.0127</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.0351</v>
+        <v>0.0161</v>
       </c>
       <c r="AC19" t="n">
-        <v>-0.0468</v>
+        <v>-0.0247</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.0727</v>
+        <v>-0.0237</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.0052</v>
+        <v>-0.028</v>
       </c>
     </row>
     <row r="20">
@@ -2246,94 +2246,94 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0039</v>
+        <v>0.167</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1792</v>
+        <v>0.1395</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1364</v>
+        <v>0.2149</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1896</v>
+        <v>0.1697</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1545</v>
+        <v>0.1794</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0247</v>
+        <v>0.1805</v>
       </c>
       <c r="H20" t="n">
-        <v>0.239</v>
+        <v>0.1533</v>
       </c>
       <c r="I20" t="n">
-        <v>0.1208</v>
+        <v>0.2313</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2234</v>
+        <v>0.1748</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0208</v>
+        <v>0.1138</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.0039</v>
+        <v>0.2096</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.0442</v>
+        <v>0.1095</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0779</v>
+        <v>0.1599</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0052</v>
+        <v>0.1737</v>
       </c>
       <c r="P20" t="n">
-        <v>0.2532</v>
+        <v>0.2332</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.1974</v>
+        <v>0.1145</v>
       </c>
       <c r="R20" t="n">
-        <v>-0.0377</v>
+        <v>0.0828</v>
       </c>
       <c r="S20" t="n">
-        <v>-0.1052</v>
+        <v>-0.0124</v>
       </c>
       <c r="T20" t="n">
         <v>1</v>
       </c>
       <c r="U20" t="n">
-        <v>0.2078</v>
+        <v>0.1217</v>
       </c>
       <c r="V20" t="n">
-        <v>-0.0058</v>
+        <v>0.0303</v>
       </c>
       <c r="W20" t="n">
-        <v>0.1468</v>
+        <v>0.1642</v>
       </c>
       <c r="X20" t="n">
-        <v>0.2</v>
+        <v>0.1665</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.0377</v>
+        <v>0.1268</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.2286</v>
+        <v>0.1665</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.074</v>
+        <v>0.1372</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.0649</v>
+        <v>0.1926</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.1442</v>
+        <v>0.137</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.0169</v>
+        <v>-0.0127</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.0636</v>
+        <v>-0.064</v>
       </c>
     </row>
     <row r="21">
@@ -2341,94 +2341,94 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2532</v>
+        <v>0.2834</v>
       </c>
       <c r="C21" t="n">
-        <v>0.013</v>
+        <v>0.0853</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2714</v>
+        <v>0.3014</v>
       </c>
       <c r="E21" t="n">
-        <v>0.1584</v>
+        <v>0.181</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3883</v>
+        <v>0.2869</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1208</v>
+        <v>0.2491</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0779</v>
+        <v>0.0331</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0532</v>
+        <v>0.1303</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2519</v>
+        <v>0.1333</v>
       </c>
       <c r="K21" t="n">
-        <v>0.1844</v>
+        <v>0.1654</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0844</v>
+        <v>0.2751</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0779</v>
+        <v>0.1813</v>
       </c>
       <c r="N21" t="n">
-        <v>0.1922</v>
+        <v>0.221</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0052</v>
+        <v>0.1474</v>
       </c>
       <c r="P21" t="n">
-        <v>0.1519</v>
+        <v>0.1216</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.1299</v>
+        <v>0.1579</v>
       </c>
       <c r="R21" t="n">
-        <v>0.0792</v>
+        <v>0.0631</v>
       </c>
       <c r="S21" t="n">
-        <v>-0.1857</v>
+        <v>-0.0406</v>
       </c>
       <c r="T21" t="n">
-        <v>0.2078</v>
+        <v>0.1217</v>
       </c>
       <c r="U21" t="n">
         <v>1</v>
       </c>
       <c r="V21" t="n">
-        <v>0.0825</v>
+        <v>0.0708</v>
       </c>
       <c r="W21" t="n">
-        <v>0.2974</v>
+        <v>0.3164</v>
       </c>
       <c r="X21" t="n">
-        <v>0.4078</v>
+        <v>0.3398</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.339</v>
+        <v>0.2276</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.2571</v>
+        <v>0.1859</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.1078</v>
+        <v>0.1004</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.1195</v>
+        <v>0.2076</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.2481</v>
+        <v>0.3042</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.1286</v>
+        <v>-0.0004</v>
       </c>
       <c r="AE21" t="n">
-        <v>-0.0195</v>
+        <v>-0.1381</v>
       </c>
     </row>
     <row r="22">
@@ -2436,94 +2436,94 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1384</v>
+        <v>0.1515</v>
       </c>
       <c r="C22" t="n">
-        <v>0.1072</v>
+        <v>0.0813</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1955</v>
+        <v>0.1159</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.0604</v>
+        <v>0.0344</v>
       </c>
       <c r="F22" t="n">
-        <v>0.141</v>
+        <v>0.0856</v>
       </c>
       <c r="G22" t="n">
-        <v>0.1773</v>
+        <v>0.1137</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.1163</v>
+        <v>-0.0072</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.1591</v>
+        <v>0.0164</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0994</v>
+        <v>0.0395</v>
       </c>
       <c r="K22" t="n">
-        <v>0.254</v>
+        <v>0.0718</v>
       </c>
       <c r="L22" t="n">
-        <v>0.1669</v>
+        <v>0.1103</v>
       </c>
       <c r="M22" t="n">
-        <v>0.1462</v>
+        <v>0.0819</v>
       </c>
       <c r="N22" t="n">
-        <v>-0.1046</v>
+        <v>0.0666</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0552</v>
+        <v>0.1016</v>
       </c>
       <c r="P22" t="n">
-        <v>0.1215</v>
+        <v>0.0424</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.2917</v>
+        <v>0.1274</v>
       </c>
       <c r="R22" t="n">
-        <v>0.1072</v>
+        <v>0.0492</v>
       </c>
       <c r="S22" t="n">
-        <v>0.0318</v>
+        <v>0.0567</v>
       </c>
       <c r="T22" t="n">
-        <v>-0.0058</v>
+        <v>0.0303</v>
       </c>
       <c r="U22" t="n">
-        <v>0.0825</v>
+        <v>0.0708</v>
       </c>
       <c r="V22" t="n">
         <v>1</v>
       </c>
       <c r="W22" t="n">
-        <v>-0.0773</v>
+        <v>0.0456</v>
       </c>
       <c r="X22" t="n">
-        <v>0.0045</v>
+        <v>0.0869</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.1202</v>
+        <v>0.0794</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.0019</v>
+        <v>0.0552</v>
       </c>
       <c r="AA22" t="n">
-        <v>-0.0526</v>
+        <v>0.0545</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.1332</v>
+        <v>0.1228</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.0188</v>
+        <v>0.0708</v>
       </c>
       <c r="AD22" t="n">
-        <v>-0.0799</v>
+        <v>-0.0508</v>
       </c>
       <c r="AE22" t="n">
-        <v>-0.202</v>
+        <v>-0.0909</v>
       </c>
     </row>
     <row r="23">
@@ -2531,94 +2531,94 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.3403</v>
+        <v>0.2907</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0429</v>
+        <v>0.1277</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3195</v>
+        <v>0.3596</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2636</v>
+        <v>0.2716</v>
       </c>
       <c r="F23" t="n">
-        <v>0.3636</v>
+        <v>0.3568</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1558</v>
+        <v>0.2727</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0532</v>
+        <v>0.0255</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2519</v>
+        <v>0.2309</v>
       </c>
       <c r="J23" t="n">
-        <v>0.2377</v>
+        <v>0.2111</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0844</v>
+        <v>0.1604</v>
       </c>
       <c r="L23" t="n">
-        <v>0.2935</v>
+        <v>0.3848</v>
       </c>
       <c r="M23" t="n">
-        <v>0.1649</v>
+        <v>0.222</v>
       </c>
       <c r="N23" t="n">
-        <v>0.3052</v>
+        <v>0.3048</v>
       </c>
       <c r="O23" t="n">
-        <v>0.2403</v>
+        <v>0.2378</v>
       </c>
       <c r="P23" t="n">
-        <v>0.1455</v>
+        <v>0.174</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.113</v>
+        <v>0.1587</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0675</v>
+        <v>0.1185</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.0286</v>
+        <v>0.009</v>
       </c>
       <c r="T23" t="n">
-        <v>0.1468</v>
+        <v>0.1642</v>
       </c>
       <c r="U23" t="n">
-        <v>0.2974</v>
+        <v>0.3164</v>
       </c>
       <c r="V23" t="n">
-        <v>-0.0773</v>
+        <v>0.0456</v>
       </c>
       <c r="W23" t="n">
         <v>1</v>
       </c>
       <c r="X23" t="n">
-        <v>0.5623</v>
+        <v>0.5039</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.439</v>
+        <v>0.2796</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.3571</v>
+        <v>0.311</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.3558</v>
+        <v>0.191</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.2143</v>
+        <v>0.2575</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.5143</v>
+        <v>0.42</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.0623</v>
+        <v>0.0249</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.0234</v>
+        <v>-0.1174</v>
       </c>
     </row>
     <row r="24">
@@ -2626,94 +2626,94 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.2818</v>
+        <v>0.3097</v>
       </c>
       <c r="C24" t="n">
-        <v>0.1169</v>
+        <v>0.1185</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3494</v>
+        <v>0.3619</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2312</v>
+        <v>0.268</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3909</v>
+        <v>0.4037</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2143</v>
+        <v>0.274</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0571</v>
+        <v>0.059</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2532</v>
+        <v>0.2134</v>
       </c>
       <c r="J24" t="n">
-        <v>0.2649</v>
+        <v>0.2185</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0987</v>
+        <v>0.1727</v>
       </c>
       <c r="L24" t="n">
-        <v>0.2506</v>
+        <v>0.3563</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0494</v>
+        <v>0.2434</v>
       </c>
       <c r="N24" t="n">
-        <v>0.2104</v>
+        <v>0.3248</v>
       </c>
       <c r="O24" t="n">
-        <v>0.1688</v>
+        <v>0.2364</v>
       </c>
       <c r="P24" t="n">
-        <v>0.1935</v>
+        <v>0.1921</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.1117</v>
+        <v>0.1913</v>
       </c>
       <c r="R24" t="n">
-        <v>0.0584</v>
+        <v>0.1332</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.1442</v>
+        <v>-0.0038</v>
       </c>
       <c r="T24" t="n">
-        <v>0.2</v>
+        <v>0.1665</v>
       </c>
       <c r="U24" t="n">
-        <v>0.4078</v>
+        <v>0.3398</v>
       </c>
       <c r="V24" t="n">
-        <v>0.0045</v>
+        <v>0.0869</v>
       </c>
       <c r="W24" t="n">
-        <v>0.5623</v>
+        <v>0.5039</v>
       </c>
       <c r="X24" t="n">
         <v>1</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.4195</v>
+        <v>0.2894</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.3065</v>
+        <v>0.3294</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.1987</v>
+        <v>0.2305</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.1636</v>
+        <v>0.2805</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.4558</v>
+        <v>0.4699</v>
       </c>
       <c r="AD24" t="n">
-        <v>-0.0506</v>
+        <v>0.008</v>
       </c>
       <c r="AE24" t="n">
-        <v>-0.0299</v>
+        <v>-0.1076</v>
       </c>
     </row>
     <row r="25">
@@ -2721,94 +2721,94 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.4052</v>
+        <v>0.2859</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0351</v>
+        <v>0.1258</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4078</v>
+        <v>0.314</v>
       </c>
       <c r="E25" t="n">
-        <v>0.2532</v>
+        <v>0.1899</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3792</v>
+        <v>0.2419</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2987</v>
+        <v>0.2994</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0117</v>
+        <v>0.0721</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2753</v>
+        <v>0.1775</v>
       </c>
       <c r="J25" t="n">
-        <v>0.1961</v>
+        <v>0.1093</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2481</v>
+        <v>0.187</v>
       </c>
       <c r="L25" t="n">
-        <v>0.4026</v>
+        <v>0.2967</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1519</v>
+        <v>0.1894</v>
       </c>
       <c r="N25" t="n">
-        <v>0.2377</v>
+        <v>0.1617</v>
       </c>
       <c r="O25" t="n">
-        <v>0.1597</v>
+        <v>0.1484</v>
       </c>
       <c r="P25" t="n">
-        <v>0.1818</v>
+        <v>0.1441</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.126</v>
+        <v>0.2282</v>
       </c>
       <c r="R25" t="n">
-        <v>0.1948</v>
+        <v>0.1014</v>
       </c>
       <c r="S25" t="n">
-        <v>-0.0468</v>
+        <v>-0.0147</v>
       </c>
       <c r="T25" t="n">
-        <v>0.0377</v>
+        <v>0.1268</v>
       </c>
       <c r="U25" t="n">
-        <v>0.339</v>
+        <v>0.2276</v>
       </c>
       <c r="V25" t="n">
-        <v>0.1202</v>
+        <v>0.0794</v>
       </c>
       <c r="W25" t="n">
-        <v>0.439</v>
+        <v>0.2796</v>
       </c>
       <c r="X25" t="n">
-        <v>0.4195</v>
+        <v>0.2894</v>
       </c>
       <c r="Y25" t="n">
         <v>1</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.2818</v>
+        <v>0.2242</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.2805</v>
+        <v>0.1657</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.1831</v>
+        <v>0.2269</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.2961</v>
+        <v>0.2597</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.1377</v>
+        <v>0.0143</v>
       </c>
       <c r="AE25" t="n">
-        <v>-0.0597</v>
+        <v>-0.1554</v>
       </c>
     </row>
     <row r="26">
@@ -2816,94 +2816,94 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.3234</v>
+        <v>0.2748</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1299</v>
+        <v>0.1632</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3701</v>
+        <v>0.3124</v>
       </c>
       <c r="E26" t="n">
-        <v>0.3221</v>
+        <v>0.3158</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1935</v>
+        <v>0.2681</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2662</v>
+        <v>0.2682</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0779</v>
+        <v>0.1259</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1286</v>
+        <v>0.2507</v>
       </c>
       <c r="J26" t="n">
-        <v>0.1792</v>
+        <v>0.1929</v>
       </c>
       <c r="K26" t="n">
-        <v>0.1195</v>
+        <v>0.2165</v>
       </c>
       <c r="L26" t="n">
-        <v>0.2325</v>
+        <v>0.2938</v>
       </c>
       <c r="M26" t="n">
-        <v>0.026</v>
+        <v>0.185</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0442</v>
+        <v>0.2399</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0857</v>
+        <v>0.2003</v>
       </c>
       <c r="P26" t="n">
-        <v>0.2948</v>
+        <v>0.2187</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.2</v>
+        <v>0.1873</v>
       </c>
       <c r="R26" t="n">
-        <v>-0.0532</v>
+        <v>0.1283</v>
       </c>
       <c r="S26" t="n">
-        <v>-0.0714</v>
+        <v>0.0076</v>
       </c>
       <c r="T26" t="n">
-        <v>0.2286</v>
+        <v>0.1665</v>
       </c>
       <c r="U26" t="n">
-        <v>0.2571</v>
+        <v>0.1859</v>
       </c>
       <c r="V26" t="n">
-        <v>0.0019</v>
+        <v>0.0552</v>
       </c>
       <c r="W26" t="n">
-        <v>0.3571</v>
+        <v>0.311</v>
       </c>
       <c r="X26" t="n">
-        <v>0.3065</v>
+        <v>0.3294</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.2818</v>
+        <v>0.2242</v>
       </c>
       <c r="Z26" t="n">
         <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.2117</v>
+        <v>0.2471</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.0675</v>
+        <v>0.22</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.1987</v>
+        <v>0.2091</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.0221</v>
+        <v>-0.0045</v>
       </c>
       <c r="AE26" t="n">
-        <v>-0.0792</v>
+        <v>-0.1106</v>
       </c>
     </row>
     <row r="27">
@@ -2911,94 +2911,94 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.239</v>
+        <v>0.1411</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0039</v>
+        <v>0.1167</v>
       </c>
       <c r="D27" t="n">
-        <v>0.1766</v>
+        <v>0.2206</v>
       </c>
       <c r="E27" t="n">
-        <v>0.1857</v>
+        <v>0.1709</v>
       </c>
       <c r="F27" t="n">
-        <v>0.2</v>
+        <v>0.1852</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0597</v>
+        <v>0.1765</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0013</v>
+        <v>0.1499</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2078</v>
+        <v>0.2459</v>
       </c>
       <c r="J27" t="n">
-        <v>0.274</v>
+        <v>0.3356</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.0195</v>
+        <v>0.0843</v>
       </c>
       <c r="L27" t="n">
-        <v>0.1636</v>
+        <v>0.1898</v>
       </c>
       <c r="M27" t="n">
-        <v>0.1468</v>
+        <v>0.1248</v>
       </c>
       <c r="N27" t="n">
-        <v>0.3545</v>
+        <v>0.2795</v>
       </c>
       <c r="O27" t="n">
-        <v>0.3675</v>
+        <v>0.388</v>
       </c>
       <c r="P27" t="n">
-        <v>0.1377</v>
+        <v>0.1659</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.0714</v>
+        <v>0.1104</v>
       </c>
       <c r="R27" t="n">
-        <v>0.1974</v>
+        <v>0.1528</v>
       </c>
       <c r="S27" t="n">
-        <v>0.0312</v>
+        <v>-0.0127</v>
       </c>
       <c r="T27" t="n">
-        <v>0.074</v>
+        <v>0.1372</v>
       </c>
       <c r="U27" t="n">
-        <v>0.1078</v>
+        <v>0.1004</v>
       </c>
       <c r="V27" t="n">
-        <v>-0.0526</v>
+        <v>0.0545</v>
       </c>
       <c r="W27" t="n">
-        <v>0.3558</v>
+        <v>0.191</v>
       </c>
       <c r="X27" t="n">
-        <v>0.1987</v>
+        <v>0.2305</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.2805</v>
+        <v>0.1657</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.2117</v>
+        <v>0.2471</v>
       </c>
       <c r="AA27" t="n">
         <v>1</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.0688</v>
+        <v>0.1659</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.1792</v>
+        <v>0.1088</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.1143</v>
+        <v>0.0319</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.0104</v>
+        <v>-0.0123</v>
       </c>
     </row>
     <row r="28">
@@ -3006,94 +3006,94 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1156</v>
+        <v>0.2543</v>
       </c>
       <c r="C28" t="n">
-        <v>0.1065</v>
+        <v>0.1642</v>
       </c>
       <c r="D28" t="n">
-        <v>0.2688</v>
+        <v>0.3089</v>
       </c>
       <c r="E28" t="n">
-        <v>0.1091</v>
+        <v>0.1821</v>
       </c>
       <c r="F28" t="n">
-        <v>0.2766</v>
+        <v>0.2251</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1935</v>
+        <v>0.2359</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0753</v>
+        <v>0.097</v>
       </c>
       <c r="I28" t="n">
-        <v>0.1597</v>
+        <v>0.1837</v>
       </c>
       <c r="J28" t="n">
-        <v>0.1662</v>
+        <v>0.1573</v>
       </c>
       <c r="K28" t="n">
-        <v>0.1558</v>
+        <v>0.2031</v>
       </c>
       <c r="L28" t="n">
-        <v>0.1961</v>
+        <v>0.2595</v>
       </c>
       <c r="M28" t="n">
-        <v>0.0675</v>
+        <v>0.1722</v>
       </c>
       <c r="N28" t="n">
-        <v>0.1896</v>
+        <v>0.2102</v>
       </c>
       <c r="O28" t="n">
-        <v>0.1013</v>
+        <v>0.1541</v>
       </c>
       <c r="P28" t="n">
-        <v>0.1701</v>
+        <v>0.1922</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.1221</v>
+        <v>0.1826</v>
       </c>
       <c r="R28" t="n">
-        <v>0.126</v>
+        <v>0.1122</v>
       </c>
       <c r="S28" t="n">
-        <v>0.0351</v>
+        <v>0.0161</v>
       </c>
       <c r="T28" t="n">
-        <v>0.0649</v>
+        <v>0.1926</v>
       </c>
       <c r="U28" t="n">
-        <v>0.1195</v>
+        <v>0.2076</v>
       </c>
       <c r="V28" t="n">
-        <v>0.1332</v>
+        <v>0.1228</v>
       </c>
       <c r="W28" t="n">
-        <v>0.2143</v>
+        <v>0.2575</v>
       </c>
       <c r="X28" t="n">
-        <v>0.1636</v>
+        <v>0.2805</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.1831</v>
+        <v>0.2269</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.0675</v>
+        <v>0.22</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.0688</v>
+        <v>0.1659</v>
       </c>
       <c r="AB28" t="n">
         <v>1</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.1961</v>
+        <v>0.2408</v>
       </c>
       <c r="AD28" t="n">
-        <v>-0.0325</v>
+        <v>-0.0314</v>
       </c>
       <c r="AE28" t="n">
-        <v>-0.0325</v>
+        <v>-0.1312</v>
       </c>
     </row>
     <row r="29">
@@ -3101,94 +3101,94 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.2519</v>
+        <v>0.2441</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1156</v>
+        <v>0.1313</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2727</v>
+        <v>0.2833</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1675</v>
+        <v>0.1863</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2857</v>
+        <v>0.2996</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1532</v>
+        <v>0.2063</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1182</v>
+        <v>-0.0112</v>
       </c>
       <c r="I29" t="n">
-        <v>0.3039</v>
+        <v>0.1307</v>
       </c>
       <c r="J29" t="n">
-        <v>0.2429</v>
+        <v>0.1206</v>
       </c>
       <c r="K29" t="n">
-        <v>0.1623</v>
+        <v>0.1599</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1948</v>
+        <v>0.2772</v>
       </c>
       <c r="M29" t="n">
-        <v>0.1468</v>
+        <v>0.2188</v>
       </c>
       <c r="N29" t="n">
-        <v>0.2532</v>
+        <v>0.2277</v>
       </c>
       <c r="O29" t="n">
-        <v>0.2013</v>
+        <v>0.1594</v>
       </c>
       <c r="P29" t="n">
-        <v>0.0649</v>
+        <v>0.1199</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.1571</v>
+        <v>0.1843</v>
       </c>
       <c r="R29" t="n">
-        <v>0.0805</v>
+        <v>0.0961</v>
       </c>
       <c r="S29" t="n">
-        <v>-0.0468</v>
+        <v>-0.0247</v>
       </c>
       <c r="T29" t="n">
-        <v>0.1442</v>
+        <v>0.137</v>
       </c>
       <c r="U29" t="n">
-        <v>0.2481</v>
+        <v>0.3042</v>
       </c>
       <c r="V29" t="n">
-        <v>0.0188</v>
+        <v>0.0708</v>
       </c>
       <c r="W29" t="n">
-        <v>0.5143</v>
+        <v>0.42</v>
       </c>
       <c r="X29" t="n">
-        <v>0.4558</v>
+        <v>0.4699</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.2961</v>
+        <v>0.2597</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.1987</v>
+        <v>0.2091</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.1792</v>
+        <v>0.1088</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.1961</v>
+        <v>0.2408</v>
       </c>
       <c r="AC29" t="n">
         <v>1</v>
       </c>
       <c r="AD29" t="n">
-        <v>-0.0052</v>
+        <v>-0.0116</v>
       </c>
       <c r="AE29" t="n">
-        <v>-0.0208</v>
+        <v>-0.1208</v>
       </c>
     </row>
     <row r="30">
@@ -3196,94 +3196,94 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.0545</v>
+        <v>-0.0433</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.2039</v>
+        <v>-0.0117</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0364</v>
+        <v>-0.0187</v>
       </c>
       <c r="E30" t="n">
-        <v>0.1208</v>
+        <v>0.0184</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0545</v>
+        <v>-0.0009</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.1948</v>
+        <v>-0.1061</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0636</v>
+        <v>0.0059</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.0234</v>
+        <v>0.0275</v>
       </c>
       <c r="J30" t="n">
-        <v>0.1597</v>
+        <v>0.0174</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.0584</v>
+        <v>0.0351</v>
       </c>
       <c r="L30" t="n">
-        <v>0.026</v>
+        <v>-0.03</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0948</v>
+        <v>-0.0154</v>
       </c>
       <c r="N30" t="n">
-        <v>0.1468</v>
+        <v>0.0251</v>
       </c>
       <c r="O30" t="n">
-        <v>0.0065</v>
+        <v>-0.0003</v>
       </c>
       <c r="P30" t="n">
-        <v>0.0571</v>
+        <v>-0.0434</v>
       </c>
       <c r="Q30" t="n">
-        <v>-0.1312</v>
+        <v>-0.0625</v>
       </c>
       <c r="R30" t="n">
-        <v>0.0649</v>
+        <v>0.0497</v>
       </c>
       <c r="S30" t="n">
-        <v>0.0727</v>
+        <v>-0.0237</v>
       </c>
       <c r="T30" t="n">
-        <v>0.0169</v>
+        <v>-0.0127</v>
       </c>
       <c r="U30" t="n">
-        <v>0.1286</v>
+        <v>-0.0004</v>
       </c>
       <c r="V30" t="n">
-        <v>-0.0799</v>
+        <v>-0.0508</v>
       </c>
       <c r="W30" t="n">
-        <v>0.0623</v>
+        <v>0.0249</v>
       </c>
       <c r="X30" t="n">
-        <v>-0.0506</v>
+        <v>0.008</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.1377</v>
+        <v>0.0143</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.0221</v>
+        <v>-0.0045</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.1143</v>
+        <v>0.0319</v>
       </c>
       <c r="AB30" t="n">
-        <v>-0.0325</v>
+        <v>-0.0314</v>
       </c>
       <c r="AC30" t="n">
-        <v>-0.0052</v>
+        <v>-0.0116</v>
       </c>
       <c r="AD30" t="n">
         <v>1</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.2104</v>
+        <v>0.2561</v>
       </c>
     </row>
     <row r="31">
@@ -3291,91 +3291,91 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.1169</v>
+        <v>-0.2017</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.0325</v>
+        <v>-0.0855</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.1662</v>
+        <v>-0.226</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.0065</v>
+        <v>-0.0845</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.0494</v>
+        <v>-0.1158</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.3065</v>
+        <v>-0.3089</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0195</v>
+        <v>-0.0088</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.026</v>
+        <v>-0.0177</v>
       </c>
       <c r="J31" t="n">
-        <v>0.0818</v>
+        <v>-0.0223</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.0143</v>
+        <v>-0.0313</v>
       </c>
       <c r="L31" t="n">
-        <v>-0.1455</v>
+        <v>-0.2095</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0117</v>
+        <v>-0.1248</v>
       </c>
       <c r="N31" t="n">
-        <v>0.2195</v>
+        <v>-0.0283</v>
       </c>
       <c r="O31" t="n">
-        <v>-0.0377</v>
+        <v>-0.063</v>
       </c>
       <c r="P31" t="n">
-        <v>-0.0312</v>
+        <v>-0.0673</v>
       </c>
       <c r="Q31" t="n">
-        <v>-0.1545</v>
+        <v>-0.1</v>
       </c>
       <c r="R31" t="n">
-        <v>0.2831</v>
+        <v>0.1188</v>
       </c>
       <c r="S31" t="n">
-        <v>0.0052</v>
+        <v>-0.028</v>
       </c>
       <c r="T31" t="n">
-        <v>0.0636</v>
+        <v>-0.064</v>
       </c>
       <c r="U31" t="n">
-        <v>-0.0195</v>
+        <v>-0.1381</v>
       </c>
       <c r="V31" t="n">
-        <v>-0.202</v>
+        <v>-0.0909</v>
       </c>
       <c r="W31" t="n">
-        <v>0.0234</v>
+        <v>-0.1174</v>
       </c>
       <c r="X31" t="n">
-        <v>-0.0299</v>
+        <v>-0.1076</v>
       </c>
       <c r="Y31" t="n">
-        <v>-0.0597</v>
+        <v>-0.1554</v>
       </c>
       <c r="Z31" t="n">
-        <v>-0.0792</v>
+        <v>-0.1106</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.0104</v>
+        <v>-0.0123</v>
       </c>
       <c r="AB31" t="n">
-        <v>-0.0325</v>
+        <v>-0.1312</v>
       </c>
       <c r="AC31" t="n">
-        <v>-0.0208</v>
+        <v>-0.1208</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.2104</v>
+        <v>0.2561</v>
       </c>
       <c r="AE31" t="n">
         <v>1</v>

</xml_diff>